<commit_message>
Fix js calendar. Fix Bożena and 'Name, Surname' in resources
</commit_message>
<xml_diff>
--- a/resources/10_audience_conflicts.xlsx
+++ b/resources/10_audience_conflicts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="31">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Physics </t>
   </si>
   <si>
-    <t xml:space="preserve">Iwaniec Joanna</t>
+    <t xml:space="preserve">Joanna Iwaniec</t>
   </si>
   <si>
     <t xml:space="preserve">2.41</t>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">3.27a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giermek Bozena</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation of Electronic Circuits</t>
@@ -245,19 +242,19 @@
   </sheetPr>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A:A"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E76" activeCellId="0" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.9433198380567"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="4" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -459,7 +456,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>1</v>
@@ -502,10 +499,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>1</v>
@@ -525,10 +522,10 @@
         <v>0.520833333333333</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>1</v>
@@ -548,10 +545,10 @@
         <v>0.604166666666667</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>1</v>
@@ -571,16 +568,16 @@
         <v>0.458333333333333</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F14" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +591,10 @@
         <v>0.534722222222222</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>2</v>
@@ -617,10 +614,10 @@
         <v>0.725694444444444</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>2</v>
@@ -640,10 +637,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>3</v>
@@ -663,10 +660,10 @@
         <v>0.618055555555556</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>3</v>
@@ -686,16 +683,16 @@
         <v>0.75</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F19" s="4" t="n">
         <v>3</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,10 +706,10 @@
         <v>0.75</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>1</v>
@@ -787,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>2</v>
@@ -925,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,10 +936,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>1</v>
@@ -962,10 +959,10 @@
         <v>0.520833333333333</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>1</v>
@@ -985,10 +982,10 @@
         <v>0.729166666666667</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>1</v>
@@ -1008,10 +1005,10 @@
         <v>0.458333333333333</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F33" s="4" t="n">
         <v>2</v>
@@ -1031,10 +1028,10 @@
         <v>0.552083333333333</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>2</v>
@@ -1054,10 +1051,10 @@
         <v>0.725694444444444</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>2</v>
@@ -1077,10 +1074,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>3</v>
@@ -1100,10 +1097,10 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F37" s="4" t="n">
         <v>3</v>
@@ -1123,10 +1120,10 @@
         <v>0.618055555555556</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F38" s="4" t="n">
         <v>3</v>
@@ -1146,10 +1143,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>1</v>
@@ -1169,10 +1166,10 @@
         <v>0.4375</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>2</v>
@@ -1238,10 +1235,10 @@
         <v>0.583333333333333</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F43" s="4" t="n">
         <v>2</v>
@@ -1284,10 +1281,10 @@
         <v>0.666666666666667</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F45" s="4" t="n">
         <v>3</v>
@@ -1307,16 +1304,16 @@
         <v>0.75</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F46" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,10 +1373,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F49" s="4" t="n">
         <v>1</v>
@@ -1399,10 +1396,10 @@
         <v>0.520833333333333</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F50" s="4" t="n">
         <v>1</v>
@@ -1422,10 +1419,10 @@
         <v>0.770833333333333</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F51" s="4" t="n">
         <v>1</v>
@@ -1445,10 +1442,10 @@
         <v>0.458333333333333</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F52" s="4" t="n">
         <v>2</v>
@@ -1468,10 +1465,10 @@
         <v>0.552083333333333</v>
       </c>
       <c r="D53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F53" s="4" t="n">
         <v>2</v>
@@ -1491,10 +1488,10 @@
         <v>0.725694444444444</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F54" s="4" t="n">
         <v>2</v>
@@ -1514,10 +1511,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F55" s="4" t="n">
         <v>3</v>
@@ -1537,10 +1534,10 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>3</v>
@@ -1560,10 +1557,10 @@
         <v>0.618055555555556</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F57" s="4" t="n">
         <v>3</v>
@@ -1629,10 +1626,10 @@
         <v>0.4375</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F60" s="4" t="n">
         <v>2</v>
@@ -1701,7 +1698,7 @@
         <v>16</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F63" s="4" t="n">
         <v>2</v>
@@ -1744,10 +1741,10 @@
         <v>0.666666666666667</v>
       </c>
       <c r="D65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F65" s="4" t="n">
         <v>3</v>
@@ -1770,7 +1767,7 @@
         <v>16</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F66" s="4" t="n">
         <v>1</v>
@@ -1836,10 +1833,10 @@
         <v>0.520833333333333</v>
       </c>
       <c r="D69" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F69" s="4" t="n">
         <v>1</v>
@@ -1859,10 +1856,10 @@
         <v>0.729166666666667</v>
       </c>
       <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F70" s="4" t="n">
         <v>1</v>
@@ -1905,10 +1902,10 @@
         <v>0.552083333333333</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F72" s="4" t="n">
         <v>2</v>
@@ -1928,10 +1925,10 @@
         <v>0.725694444444444</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F73" s="4" t="n">
         <v>2</v>
@@ -1951,10 +1948,10 @@
         <v>0.416666666666667</v>
       </c>
       <c r="D74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F74" s="4" t="n">
         <v>3</v>
@@ -1974,10 +1971,10 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F75" s="4" t="n">
         <v>3</v>
@@ -2028,7 +2025,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2054,7 +2051,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>